<commit_message>
full trade pull finished
</commit_message>
<xml_diff>
--- a/KXMARMAD_events.xlsx
+++ b/KXMARMAD_events.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="12" documentId="11_4BF173BAD3F05E25B7192D11595ED87656CD632C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8EB22758-8F85-4E41-88D2-8E566DA7D2E6}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -859,8 +859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="M59" sqref="M59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>